<commit_message>
modified task_2, separated the controller layer, handled inner function errs, fixed postman collection
</commit_message>
<xml_diff>
--- a/Growpital_backend_task_2.xlsx
+++ b/Growpital_backend_task_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meta\Desktop\GrowPital Backend Challenge\Task 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meta\Desktop\GrowPital Backend Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E99B7E-1D21-4C28-BD6D-04C0A2AE211B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457F1F3D-6175-425B-8D40-54237BF93DE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Widget</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>/wallet/depost</t>
-  </si>
-  <si>
-    <t>/wallet/transactions</t>
   </si>
   <si>
     <t>Response (Pending)</t>
@@ -109,9 +106,6 @@
     <t>Important</t>
   </si>
   <si>
-    <t>{ "transaction_id": "DBTR/222201998174"  }</t>
-  </si>
-  <si>
     <t>{ name: "Saurabh Sharma",
 customer_id: "some_unique_id",
 amount: "15000" 
@@ -131,6 +125,15 @@
   </si>
   <si>
     <t xml:space="preserve">The second api is called only when the user wants to know about the transaction/ or some other transaction after some time or after logging out </t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>/wallet/transactions/:transaction_id</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
   <dimension ref="A1:AA969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -589,7 +592,7 @@
     <col min="1" max="1" width="10.5703125" style="3" customWidth="1"/>
     <col min="2" max="3" width="12.5703125" style="3"/>
     <col min="4" max="4" width="27.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="65.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -601,7 +604,7 @@
     <row r="1" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="D1" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
@@ -625,7 +628,7 @@
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D2" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
@@ -633,7 +636,7 @@
     </row>
     <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D3" s="24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
@@ -673,10 +676,10 @@
         <v>5</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>6</v>
@@ -714,47 +717,47 @@
         <v>10</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="15" t="s">
-        <v>15</v>
-      </c>
       <c r="J7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>